<commit_message>
Ajout du Global Transfer dans le jeu de donnée pour PNE_PHASE_01
</commit_message>
<xml_diff>
--- a/SQL Phasing Data Set.xlsx
+++ b/SQL Phasing Data Set.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ts.accenture.com/sites/PropaleSIRHCrditAgricoleS.A/Shared Documents/CASA - PROJECT/99 - Inputs Document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ts.accenture.com/sites/PropaleSIRHCrditAgricoleS.A/Shared Documents/CASA - PROJECT/20 - ITERATIONS/70 - SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60190B4F-584E-4B01-8B0A-C4A90B97FF80}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{2ADE22ED-E77A-4EBA-A1BF-865D1883EB80}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
   <si>
     <t>assignment</t>
   </si>
@@ -104,23 +104,29 @@
   </si>
   <si>
     <t>Cash Management</t>
+  </si>
+  <si>
+    <t>CREDIT AGRICOLE CIB France</t>
+  </si>
+  <si>
+    <t>CACIB</t>
+  </si>
+  <si>
+    <t>CACEIS Bank</t>
+  </si>
+  <si>
+    <t>Trader</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF707070"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -168,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -178,7 +184,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -562,34 +567,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A23D1E-6F82-4B60-90AE-0CDB18036C4E}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="16.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="1.36328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="1.36328125" style="7" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.36328125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="1.36328125" style="7" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.36328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="1.36328125" style="7" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.36328125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" style="7" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.36328125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" style="7" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.36328125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="1.36328125" style="7" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="1.36328125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="1.36328125" style="7" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.36328125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="1.36328125" style="7" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.36328125" style="7" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -617,8 +624,11 @@
       <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -649,284 +659,349 @@
       <c r="R2" s="4">
         <v>44601</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="T2" s="4">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="T5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="7"/>
+      <c r="T6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="T7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="6" t="s">
+      <c r="K8" s="7"/>
+      <c r="L8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="6" t="s">
+      <c r="M8" s="7"/>
+      <c r="N8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="6" t="s">
+      <c r="O8" s="7"/>
+      <c r="P8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="6" t="s">
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="S8" s="7"/>
+      <c r="T8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6">
+      <c r="C9" s="7"/>
+      <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6">
+      <c r="E9" s="7"/>
+      <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6">
+      <c r="G9" s="7"/>
+      <c r="H9" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="6">
+      <c r="I9" s="7"/>
+      <c r="J9" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="6">
+      <c r="K9" s="7"/>
+      <c r="L9" s="5">
         <v>1</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="6">
+      <c r="M9" s="7"/>
+      <c r="N9" s="5">
         <v>1</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="6">
+      <c r="O9" s="7"/>
+      <c r="P9" s="5">
         <v>1</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="6">
+      <c r="Q9" s="7"/>
+      <c r="R9" s="5">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="S9" s="7"/>
+      <c r="T9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>50000</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>50000</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>50000</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H10" s="3">
         <v>50000</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J10" s="3">
         <v>50000</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L10" s="3">
         <v>50000</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N10" s="3">
         <v>50000</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P10" s="3">
         <v>50000</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R10" s="3">
         <v>50000</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="T10" s="3">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1180,15 +1255,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2b399ba-b933-4889-9c1e-55eadf04d47b">
@@ -1199,14 +1265,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2A02EF4-3188-48A0-8DE0-61061D48ACF1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2A02EF4-3188-48A0-8DE0-61061D48ACF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
+    <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B80ABA-17CE-4641-ABAF-5CE41CB91BE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
+    <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B80ABA-17CE-4641-ABAF-5CE41CB91BE3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
/*gérer le passage à une autre et depuis une autre entité Groupe-->DONE*/
</commit_message>
<xml_diff>
--- a/SQL Phasing Data Set.xlsx
+++ b/SQL Phasing Data Set.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ts.accenture.com/sites/PropaleSIRHCrditAgricoleS.A/Shared Documents/CASA - PROJECT/20 - ITERATIONS/70 - SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60190B4F-584E-4B01-8B0A-C4A90B97FF80}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2AED0FC-7C9A-4CA5-B936-B47F2F402994}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{2ADE22ED-E77A-4EBA-A1BF-865D1883EB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TRIPARTITE PHASE5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
   <si>
     <t>assignment</t>
   </si>
@@ -116,16 +117,47 @@
   </si>
   <si>
     <t>Trader</t>
+  </si>
+  <si>
+    <t>PNE_PHASE_05</t>
+  </si>
+  <si>
+    <t>DET - AMUNDI</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>HIRE</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>MIG</t>
+  </si>
+  <si>
+    <t>TERMINATION</t>
+  </si>
+  <si>
+    <t>MOG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -174,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -189,6 +221,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,10 +602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A23D1E-6F82-4B60-90AE-0CDB18036C4E}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,74 +629,526 @@
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="1.36328125" style="7" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.36328125" style="7" customWidth="1"/>
+    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44531</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44531</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44593</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44597</v>
+      </c>
+      <c r="J2" s="4">
+        <v>44597</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44598</v>
+      </c>
+      <c r="N2" s="4">
+        <v>44601</v>
+      </c>
+      <c r="P2" s="4">
+        <v>44601</v>
+      </c>
+      <c r="R2" s="4">
+        <v>44602</v>
+      </c>
+      <c r="T2" s="4">
+        <v>44667</v>
+      </c>
+      <c r="V2" s="4">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="7"/>
+      <c r="T6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="7"/>
+      <c r="V6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="7"/>
+      <c r="T8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" s="7"/>
+      <c r="V8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="S9" s="7"/>
+      <c r="T9" s="5">
+        <v>1</v>
+      </c>
+      <c r="U9" s="7"/>
+      <c r="V9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="H10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="J10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="N10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="P10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="R10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="T10" s="3">
+        <v>70000</v>
+      </c>
+      <c r="V10" s="3">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48D361D-2F33-4F44-97C7-36E098ABADE2}">
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="16.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.36328125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="1.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.36328125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.36328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.36328125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.36328125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.36328125" style="7" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>2</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="4">
-        <v>44531</v>
+        <v>44600</v>
       </c>
       <c r="D2" s="4">
-        <v>44531</v>
-      </c>
-      <c r="F2" s="4">
-        <v>44593</v>
-      </c>
-      <c r="H2" s="4">
-        <v>44597</v>
-      </c>
-      <c r="J2" s="4">
-        <v>44597</v>
-      </c>
-      <c r="L2" s="4">
-        <v>44598</v>
-      </c>
-      <c r="N2" s="4">
-        <v>44601</v>
-      </c>
-      <c r="P2" s="4">
-        <v>44601</v>
-      </c>
-      <c r="R2" s="4">
-        <v>44601</v>
-      </c>
-      <c r="T2" s="4">
-        <v>44849</v>
-      </c>
+        <v>44835</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -673,337 +1160,215 @@
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="F3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="J8" s="5"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="L8" s="5"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="N8" s="5"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="P8" s="5"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="R8" s="5"/>
       <c r="S8" s="7"/>
-      <c r="T8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="5">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="5">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B12" s="3">
         <v>50000</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D12" s="3">
         <v>50000</v>
       </c>
-      <c r="F10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="H10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="J10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="L10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="N10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="P10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="R10" s="3">
-        <v>50000</v>
-      </c>
-      <c r="T10" s="3">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="T13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1255,6 +1620,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2b399ba-b933-4889-9c1e-55eadf04d47b">
@@ -1265,20 +1639,34 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF54618-FA83-480A-8389-F5A08895B168}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF54618-FA83-480A-8389-F5A08895B168}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
+    <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B80ABA-17CE-4641-ABAF-5CE41CB91BE3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1287,12 +1675,4 @@
     <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
AJOUT DES PERSONNEL IDENTIFIE ET DES DIRECTEURS
</commit_message>
<xml_diff>
--- a/SQL Phasing Data Set.xlsx
+++ b/SQL Phasing Data Set.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ts.accenture.com/sites/PropaleSIRHCrditAgricoleS.A/Shared Documents/CASA - PROJECT/20 - ITERATIONS/70 - SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2AED0FC-7C9A-4CA5-B936-B47F2F402994}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{50BF537C-32FE-4031-8E25-61E88C964689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{356931AB-2D54-4787-B738-98A2B6A8DB9E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{2ADE22ED-E77A-4EBA-A1BF-865D1883EB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="TRIPARTITE PHASE5" sheetId="3" r:id="rId3"/>
+    <sheet name="MANY MOVE &amp; C1" sheetId="2" r:id="rId2"/>
+    <sheet name="TRIPARTITE ENTRE DEPART" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="47">
   <si>
     <t>assignment</t>
   </si>
@@ -141,6 +142,42 @@
   </si>
   <si>
     <t>MOG</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>CONTRACT CHANGE</t>
+  </si>
+  <si>
+    <t>80000USD</t>
+  </si>
+  <si>
+    <t>si C1 = 14/10</t>
+  </si>
+  <si>
+    <t>sinon = 31/12</t>
+  </si>
+  <si>
+    <t>si C1 = 15/04/2022</t>
+  </si>
+  <si>
+    <t>sinon 07/07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> si C1</t>
+  </si>
+  <si>
+    <t>CREDIT AGRICOLE CIB TOKYO BRANCH</t>
+  </si>
+  <si>
+    <t>PNE_PHASE_06</t>
+  </si>
+  <si>
+    <t>100000JPY</t>
+  </si>
+  <si>
+    <t>60000eur</t>
   </si>
 </sst>
 </file>
@@ -206,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -222,6 +259,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -538,6 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A1E580-B536-422A-AC88-180A9ECAC6AD}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -602,10 +649,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A23D1E-6F82-4B60-90AE-0CDB18036C4E}">
-  <dimension ref="A1:V11"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,14 +674,18 @@
     <col min="15" max="15" width="1.36328125" style="7" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="1.36328125" style="7" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7265625" customWidth="1"/>
     <col min="19" max="19" width="1.36328125" style="7" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="1.36328125" style="7" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.36328125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.36328125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -667,8 +719,14 @@
       <c r="V1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -700,13 +758,19 @@
         <v>44602</v>
       </c>
       <c r="T2" s="4">
+        <v>44602</v>
+      </c>
+      <c r="V2" s="4">
         <v>44667</v>
       </c>
-      <c r="V2" s="4">
+      <c r="X2" s="4">
+        <v>44749</v>
+      </c>
+      <c r="Z2" s="4">
         <v>44849</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -738,13 +802,19 @@
         <v>8</v>
       </c>
       <c r="T3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -776,13 +846,19 @@
         <v>3</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -819,8 +895,14 @@
       <c r="V5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="X5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -867,8 +949,16 @@
       <c r="V6" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W6" s="7"/>
+      <c r="X6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -900,13 +990,19 @@
         <v>10</v>
       </c>
       <c r="T7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="Z7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -947,14 +1043,22 @@
       </c>
       <c r="S8" s="7"/>
       <c r="T8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" s="7"/>
+      <c r="X8" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -995,14 +1099,22 @@
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="W9" s="7"/>
+      <c r="X9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -1034,13 +1146,19 @@
         <v>50000</v>
       </c>
       <c r="T10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="V10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z10" s="3">
         <v>70000</v>
       </c>
-      <c r="V10" s="3">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1076,6 +1194,72 @@
       </c>
       <c r="V11" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="T12" s="3"/>
+      <c r="V12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="4">
+        <v>44562</v>
+      </c>
+      <c r="H13" s="4">
+        <v>44597</v>
+      </c>
+      <c r="P13" s="4">
+        <v>44601</v>
+      </c>
+      <c r="R13" s="4">
+        <v>44602</v>
+      </c>
+      <c r="V13" s="4">
+        <v>44667</v>
+      </c>
+      <c r="X13" s="4">
+        <v>44749</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="4">
+        <v>44596</v>
+      </c>
+      <c r="H14" s="4">
+        <v>44600</v>
+      </c>
+      <c r="P14" s="4">
+        <v>44601</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14" s="4">
+        <v>44748</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>1027428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="R15" t="s">
+        <v>41</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1086,10 +1270,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48D361D-2F33-4F44-97C7-36E098ABADE2}">
-  <dimension ref="A1:T13"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,9 +1283,9 @@
     <col min="3" max="3" width="1.36328125" style="7" customWidth="1"/>
     <col min="4" max="4" width="16.81640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="1.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="1.36328125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="1.36328125" style="7" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.36328125" style="7" customWidth="1"/>
@@ -1113,153 +1298,179 @@
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="1.36328125" style="7" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.36328125" style="7" customWidth="1"/>
+    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="L1" s="3"/>
       <c r="N1" s="3"/>
       <c r="P1" s="3"/>
       <c r="R1" s="3"/>
       <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="4">
+        <v>38169</v>
+      </c>
+      <c r="D2" s="4">
         <v>44600</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F2" s="4">
+        <v>44606</v>
+      </c>
+      <c r="H2" s="10">
         <v>44835</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4"/>
       <c r="J2" s="4"/>
       <c r="L2" s="4"/>
       <c r="N2" s="4"/>
       <c r="P2" s="4"/>
       <c r="R2" s="4"/>
       <c r="T2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="L3" s="4"/>
       <c r="N3" s="4"/>
       <c r="P3" s="4"/>
       <c r="R3" s="4"/>
       <c r="T3" s="4"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="H4" s="4"/>
       <c r="J4" s="4"/>
       <c r="L4" s="4"/>
       <c r="N4" s="4"/>
       <c r="P4" s="4"/>
       <c r="R4" s="4"/>
       <c r="T4" s="4"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="L5" s="4"/>
       <c r="N5" s="4"/>
       <c r="P5" s="4"/>
       <c r="R5" s="4"/>
       <c r="T5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="L6" s="3"/>
       <c r="N6" s="3"/>
       <c r="P6" s="3"/>
       <c r="R6" s="3"/>
       <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="L7" s="3"/>
       <c r="N7" s="3"/>
       <c r="P7" s="3"/>
       <c r="R7" s="3"/>
       <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="7"/>
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="5"/>
       <c r="K8" s="7"/>
@@ -1272,35 +1483,39 @@
       <c r="R8" s="5"/>
       <c r="S8" s="7"/>
       <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="7"/>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="9"/>
       <c r="J9" s="3"/>
       <c r="L9" s="3"/>
       <c r="N9" s="3"/>
       <c r="P9" s="3"/>
       <c r="R9" s="3"/>
       <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="5"/>
       <c r="K10" s="7"/>
@@ -1313,8 +1528,10 @@
       <c r="R10" s="5"/>
       <c r="S10" s="7"/>
       <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U10" s="7"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1541,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="5"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="7"/>
       <c r="J11" s="5"/>
       <c r="K11" s="7"/>
@@ -1337,38 +1554,48 @@
       <c r="R11" s="5"/>
       <c r="S11" s="7"/>
       <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U11" s="7"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
-        <v>50000</v>
-      </c>
       <c r="D12" s="3">
         <v>50000</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="F12" s="3">
+        <v>50000</v>
+      </c>
+      <c r="H12" s="9">
+        <v>50000</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="L12" s="3"/>
       <c r="N12" s="3"/>
       <c r="P12" s="3"/>
       <c r="R12" s="3"/>
       <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="9"/>
       <c r="J13" s="3"/>
       <c r="L13" s="3"/>
       <c r="N13" s="3"/>
       <c r="P13" s="3"/>
       <c r="R13" s="3"/>
       <c r="T13" s="3"/>
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1376,7 +1603,259 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B9336-7EF8-4989-B6F4-38DAB097B3C2}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="16.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.36328125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.36328125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.36328125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.36328125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.36328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4">
+        <v>43656</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44603</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f>B3</f>
+        <v>CACIB</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2b399ba-b933-4889-9c1e-55eadf04d47b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d5591cfa-a62e-4600-a72b-36d30eea89b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F715DF305527F449F9136069514364E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cb93e97eb41cdb2c39a8069c56829dcd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2b399ba-b933-4889-9c1e-55eadf04d47b" xmlns:ns3="d5591cfa-a62e-4600-a72b-36d30eea89b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6857bab30caf28c5b10026451a11661a" ns2:_="" ns3:_="">
     <xsd:import namespace="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
@@ -1619,27 +2098,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B80ABA-17CE-4641-ABAF-5CE41CB91BE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
+    <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2b399ba-b933-4889-9c1e-55eadf04d47b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d5591cfa-a62e-4600-a72b-36d30eea89b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF54618-FA83-480A-8389-F5A08895B168}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1656,23 +2134,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5311AE0-DB4C-410B-BE4C-C2B0A6A0ECBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B80ABA-17CE-4641-ABAF-5CE41CB91BE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b2b399ba-b933-4889-9c1e-55eadf04d47b"/>
-    <ds:schemaRef ds:uri="d5591cfa-a62e-4600-a72b-36d30eea89b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>